<commit_message>
New Sprite + Update
Created a Turkish Pine Sprite, updated the checklist and olive tree.
</commit_message>
<xml_diff>
--- a/LandInvaders_Artists_Checklist.xlsx
+++ b/LandInvaders_Artists_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayde\Documents\GitHub\LandInvaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6775AE00-554C-46A5-BB69-650C24700998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFA7BBD-49CE-462E-8201-1E87DCCFB7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="37695" windowHeight="21840" xr2:uid="{07534024-D62A-4DC5-98BC-199FB55393F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>Objects to Design</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Warrior</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarissa </t>
-  </si>
-  <si>
     <t>Archer</t>
   </si>
   <si>
@@ -187,6 +184,24 @@
   </si>
   <si>
     <t>Charioteer</t>
+  </si>
+  <si>
+    <t>Blocking</t>
+  </si>
+  <si>
+    <t>REDESIGN/RESIZE</t>
+  </si>
+  <si>
+    <t>Resize</t>
+  </si>
+  <si>
+    <t>Sarissa (Spear)</t>
+  </si>
+  <si>
+    <t>Ready for Placeholder</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -575,7 +590,7 @@
   <dimension ref="B4:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +598,7 @@
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" customWidth="1"/>
     <col min="10" max="10" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,7 +635,7 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -634,13 +649,13 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -651,7 +666,7 @@
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -665,13 +680,13 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -681,6 +696,18 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -689,6 +716,15 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -697,6 +733,14 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -753,21 +797,33 @@
       <c r="B27" t="s">
         <v>33</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>34</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>44</v>
       </c>
+      <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>45</v>
       </c>
+      <c r="C30" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
@@ -792,7 +848,7 @@
         <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -800,7 +856,7 @@
         <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -808,7 +864,7 @@
         <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -826,7 +882,7 @@
         <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>